<commit_message>
done code + report file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tran Phu Quy\Downloads\tk.doraneko.pcgt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E23208-C5A7-4E31-B36A-9AFA779081C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827BAE94-13B3-49FB-858F-693D5F76FFAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1350" windowWidth="15375" windowHeight="8325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GT" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="440">
   <si>
     <t>Số Thẻ</t>
   </si>
@@ -666,6 +666,681 @@
   </si>
   <si>
     <t>K51</t>
+  </si>
+  <si>
+    <t>B052</t>
+  </si>
+  <si>
+    <t>L052</t>
+  </si>
+  <si>
+    <t>K52</t>
+  </si>
+  <si>
+    <t>B053</t>
+  </si>
+  <si>
+    <t>L053</t>
+  </si>
+  <si>
+    <t>K53</t>
+  </si>
+  <si>
+    <t>B054</t>
+  </si>
+  <si>
+    <t>L054</t>
+  </si>
+  <si>
+    <t>K54</t>
+  </si>
+  <si>
+    <t>B055</t>
+  </si>
+  <si>
+    <t>L055</t>
+  </si>
+  <si>
+    <t>K55</t>
+  </si>
+  <si>
+    <t>B056</t>
+  </si>
+  <si>
+    <t>L056</t>
+  </si>
+  <si>
+    <t>K56</t>
+  </si>
+  <si>
+    <t>B057</t>
+  </si>
+  <si>
+    <t>L057</t>
+  </si>
+  <si>
+    <t>K57</t>
+  </si>
+  <si>
+    <t>B058</t>
+  </si>
+  <si>
+    <t>L058</t>
+  </si>
+  <si>
+    <t>K58</t>
+  </si>
+  <si>
+    <t>B059</t>
+  </si>
+  <si>
+    <t>L059</t>
+  </si>
+  <si>
+    <t>K59</t>
+  </si>
+  <si>
+    <t>B060</t>
+  </si>
+  <si>
+    <t>L060</t>
+  </si>
+  <si>
+    <t>K60</t>
+  </si>
+  <si>
+    <t>B061</t>
+  </si>
+  <si>
+    <t>L061</t>
+  </si>
+  <si>
+    <t>K61</t>
+  </si>
+  <si>
+    <t>B062</t>
+  </si>
+  <si>
+    <t>L062</t>
+  </si>
+  <si>
+    <t>K62</t>
+  </si>
+  <si>
+    <t>B063</t>
+  </si>
+  <si>
+    <t>L063</t>
+  </si>
+  <si>
+    <t>K63</t>
+  </si>
+  <si>
+    <t>B064</t>
+  </si>
+  <si>
+    <t>L064</t>
+  </si>
+  <si>
+    <t>K64</t>
+  </si>
+  <si>
+    <t>B065</t>
+  </si>
+  <si>
+    <t>L065</t>
+  </si>
+  <si>
+    <t>K65</t>
+  </si>
+  <si>
+    <t>B066</t>
+  </si>
+  <si>
+    <t>L066</t>
+  </si>
+  <si>
+    <t>K66</t>
+  </si>
+  <si>
+    <t>B067</t>
+  </si>
+  <si>
+    <t>L067</t>
+  </si>
+  <si>
+    <t>K67</t>
+  </si>
+  <si>
+    <t>B068</t>
+  </si>
+  <si>
+    <t>L068</t>
+  </si>
+  <si>
+    <t>K68</t>
+  </si>
+  <si>
+    <t>B069</t>
+  </si>
+  <si>
+    <t>L069</t>
+  </si>
+  <si>
+    <t>K69</t>
+  </si>
+  <si>
+    <t>B070</t>
+  </si>
+  <si>
+    <t>L070</t>
+  </si>
+  <si>
+    <t>K70</t>
+  </si>
+  <si>
+    <t>B071</t>
+  </si>
+  <si>
+    <t>L071</t>
+  </si>
+  <si>
+    <t>K71</t>
+  </si>
+  <si>
+    <t>B072</t>
+  </si>
+  <si>
+    <t>L072</t>
+  </si>
+  <si>
+    <t>K72</t>
+  </si>
+  <si>
+    <t>B073</t>
+  </si>
+  <si>
+    <t>L073</t>
+  </si>
+  <si>
+    <t>K73</t>
+  </si>
+  <si>
+    <t>B074</t>
+  </si>
+  <si>
+    <t>L074</t>
+  </si>
+  <si>
+    <t>K74</t>
+  </si>
+  <si>
+    <t>B075</t>
+  </si>
+  <si>
+    <t>L075</t>
+  </si>
+  <si>
+    <t>K75</t>
+  </si>
+  <si>
+    <t>B076</t>
+  </si>
+  <si>
+    <t>L076</t>
+  </si>
+  <si>
+    <t>K76</t>
+  </si>
+  <si>
+    <t>B077</t>
+  </si>
+  <si>
+    <t>L077</t>
+  </si>
+  <si>
+    <t>K77</t>
+  </si>
+  <si>
+    <t>B078</t>
+  </si>
+  <si>
+    <t>L078</t>
+  </si>
+  <si>
+    <t>K78</t>
+  </si>
+  <si>
+    <t>B079</t>
+  </si>
+  <si>
+    <t>L079</t>
+  </si>
+  <si>
+    <t>K79</t>
+  </si>
+  <si>
+    <t>B080</t>
+  </si>
+  <si>
+    <t>L080</t>
+  </si>
+  <si>
+    <t>K80</t>
+  </si>
+  <si>
+    <t>B081</t>
+  </si>
+  <si>
+    <t>L081</t>
+  </si>
+  <si>
+    <t>K81</t>
+  </si>
+  <si>
+    <t>B082</t>
+  </si>
+  <si>
+    <t>L082</t>
+  </si>
+  <si>
+    <t>K82</t>
+  </si>
+  <si>
+    <t>B083</t>
+  </si>
+  <si>
+    <t>L083</t>
+  </si>
+  <si>
+    <t>K83</t>
+  </si>
+  <si>
+    <t>B084</t>
+  </si>
+  <si>
+    <t>L084</t>
+  </si>
+  <si>
+    <t>K84</t>
+  </si>
+  <si>
+    <t>B085</t>
+  </si>
+  <si>
+    <t>L085</t>
+  </si>
+  <si>
+    <t>K85</t>
+  </si>
+  <si>
+    <t>B086</t>
+  </si>
+  <si>
+    <t>L086</t>
+  </si>
+  <si>
+    <t>K86</t>
+  </si>
+  <si>
+    <t>B087</t>
+  </si>
+  <si>
+    <t>L087</t>
+  </si>
+  <si>
+    <t>K87</t>
+  </si>
+  <si>
+    <t>B088</t>
+  </si>
+  <si>
+    <t>L088</t>
+  </si>
+  <si>
+    <t>K88</t>
+  </si>
+  <si>
+    <t>B089</t>
+  </si>
+  <si>
+    <t>L089</t>
+  </si>
+  <si>
+    <t>K89</t>
+  </si>
+  <si>
+    <t>B090</t>
+  </si>
+  <si>
+    <t>L090</t>
+  </si>
+  <si>
+    <t>K90</t>
+  </si>
+  <si>
+    <t>B091</t>
+  </si>
+  <si>
+    <t>L091</t>
+  </si>
+  <si>
+    <t>K91</t>
+  </si>
+  <si>
+    <t>B092</t>
+  </si>
+  <si>
+    <t>L092</t>
+  </si>
+  <si>
+    <t>K92</t>
+  </si>
+  <si>
+    <t>B093</t>
+  </si>
+  <si>
+    <t>L093</t>
+  </si>
+  <si>
+    <t>K93</t>
+  </si>
+  <si>
+    <t>B094</t>
+  </si>
+  <si>
+    <t>L094</t>
+  </si>
+  <si>
+    <t>K94</t>
+  </si>
+  <si>
+    <t>B095</t>
+  </si>
+  <si>
+    <t>L095</t>
+  </si>
+  <si>
+    <t>K95</t>
+  </si>
+  <si>
+    <t>B096</t>
+  </si>
+  <si>
+    <t>L096</t>
+  </si>
+  <si>
+    <t>K96</t>
+  </si>
+  <si>
+    <t>B097</t>
+  </si>
+  <si>
+    <t>L097</t>
+  </si>
+  <si>
+    <t>K97</t>
+  </si>
+  <si>
+    <t>B098</t>
+  </si>
+  <si>
+    <t>L098</t>
+  </si>
+  <si>
+    <t>K98</t>
+  </si>
+  <si>
+    <t>B099</t>
+  </si>
+  <si>
+    <t>L099</t>
+  </si>
+  <si>
+    <t>K99</t>
+  </si>
+  <si>
+    <t>B100</t>
+  </si>
+  <si>
+    <t>L100</t>
+  </si>
+  <si>
+    <t>K100</t>
+  </si>
+  <si>
+    <t>B101</t>
+  </si>
+  <si>
+    <t>L101</t>
+  </si>
+  <si>
+    <t>K101</t>
+  </si>
+  <si>
+    <t>B102</t>
+  </si>
+  <si>
+    <t>L102</t>
+  </si>
+  <si>
+    <t>K102</t>
+  </si>
+  <si>
+    <t>B103</t>
+  </si>
+  <si>
+    <t>L103</t>
+  </si>
+  <si>
+    <t>K103</t>
+  </si>
+  <si>
+    <t>B104</t>
+  </si>
+  <si>
+    <t>L104</t>
+  </si>
+  <si>
+    <t>K104</t>
+  </si>
+  <si>
+    <t>B105</t>
+  </si>
+  <si>
+    <t>L105</t>
+  </si>
+  <si>
+    <t>K105</t>
+  </si>
+  <si>
+    <t>B106</t>
+  </si>
+  <si>
+    <t>L106</t>
+  </si>
+  <si>
+    <t>K106</t>
+  </si>
+  <si>
+    <t>B107</t>
+  </si>
+  <si>
+    <t>L107</t>
+  </si>
+  <si>
+    <t>K107</t>
+  </si>
+  <si>
+    <t>B108</t>
+  </si>
+  <si>
+    <t>L108</t>
+  </si>
+  <si>
+    <t>K108</t>
+  </si>
+  <si>
+    <t>B109</t>
+  </si>
+  <si>
+    <t>L109</t>
+  </si>
+  <si>
+    <t>K109</t>
+  </si>
+  <si>
+    <t>B110</t>
+  </si>
+  <si>
+    <t>L110</t>
+  </si>
+  <si>
+    <t>K110</t>
+  </si>
+  <si>
+    <t>B111</t>
+  </si>
+  <si>
+    <t>L111</t>
+  </si>
+  <si>
+    <t>K111</t>
+  </si>
+  <si>
+    <t>B112</t>
+  </si>
+  <si>
+    <t>L112</t>
+  </si>
+  <si>
+    <t>K112</t>
+  </si>
+  <si>
+    <t>B113</t>
+  </si>
+  <si>
+    <t>L113</t>
+  </si>
+  <si>
+    <t>K113</t>
+  </si>
+  <si>
+    <t>B114</t>
+  </si>
+  <si>
+    <t>L114</t>
+  </si>
+  <si>
+    <t>K114</t>
+  </si>
+  <si>
+    <t>B115</t>
+  </si>
+  <si>
+    <t>L115</t>
+  </si>
+  <si>
+    <t>K115</t>
+  </si>
+  <si>
+    <t>B116</t>
+  </si>
+  <si>
+    <t>L116</t>
+  </si>
+  <si>
+    <t>K116</t>
+  </si>
+  <si>
+    <t>B117</t>
+  </si>
+  <si>
+    <t>L117</t>
+  </si>
+  <si>
+    <t>K117</t>
+  </si>
+  <si>
+    <t>B118</t>
+  </si>
+  <si>
+    <t>L118</t>
+  </si>
+  <si>
+    <t>K118</t>
+  </si>
+  <si>
+    <t>B119</t>
+  </si>
+  <si>
+    <t>L119</t>
+  </si>
+  <si>
+    <t>K119</t>
+  </si>
+  <si>
+    <t>B120</t>
+  </si>
+  <si>
+    <t>L120</t>
+  </si>
+  <si>
+    <t>K120</t>
+  </si>
+  <si>
+    <t>B121</t>
+  </si>
+  <si>
+    <t>L121</t>
+  </si>
+  <si>
+    <t>K121</t>
+  </si>
+  <si>
+    <t>B122</t>
+  </si>
+  <si>
+    <t>L122</t>
+  </si>
+  <si>
+    <t>K122</t>
+  </si>
+  <si>
+    <t>B123</t>
+  </si>
+  <si>
+    <t>L123</t>
+  </si>
+  <si>
+    <t>K123</t>
+  </si>
+  <si>
+    <t>B124</t>
+  </si>
+  <si>
+    <t>L124</t>
+  </si>
+  <si>
+    <t>K124</t>
+  </si>
+  <si>
+    <t>B125</t>
+  </si>
+  <si>
+    <t>L125</t>
+  </si>
+  <si>
+    <t>K125</t>
+  </si>
+  <si>
+    <t>B126</t>
+  </si>
+  <si>
+    <t>L126</t>
+  </si>
+  <si>
+    <t>K126</t>
   </si>
 </sst>
 </file>
@@ -1457,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,6 +2716,831 @@
         <v>214</v>
       </c>
     </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>221</v>
+      </c>
+      <c r="B55" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>224</v>
+      </c>
+      <c r="B56" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" t="s">
+        <v>228</v>
+      </c>
+      <c r="C57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>231</v>
+      </c>
+      <c r="C58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>233</v>
+      </c>
+      <c r="B59" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>242</v>
+      </c>
+      <c r="B62" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>245</v>
+      </c>
+      <c r="B63" t="s">
+        <v>246</v>
+      </c>
+      <c r="C63" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>248</v>
+      </c>
+      <c r="B64" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>254</v>
+      </c>
+      <c r="B66" t="s">
+        <v>255</v>
+      </c>
+      <c r="C66" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>257</v>
+      </c>
+      <c r="B67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>260</v>
+      </c>
+      <c r="B68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>266</v>
+      </c>
+      <c r="B70" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>269</v>
+      </c>
+      <c r="B71" t="s">
+        <v>270</v>
+      </c>
+      <c r="C71" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>272</v>
+      </c>
+      <c r="B72" t="s">
+        <v>273</v>
+      </c>
+      <c r="C72" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>275</v>
+      </c>
+      <c r="B73" t="s">
+        <v>276</v>
+      </c>
+      <c r="C73" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>278</v>
+      </c>
+      <c r="B74" t="s">
+        <v>279</v>
+      </c>
+      <c r="C74" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>281</v>
+      </c>
+      <c r="B75" t="s">
+        <v>282</v>
+      </c>
+      <c r="C75" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>284</v>
+      </c>
+      <c r="B76" t="s">
+        <v>285</v>
+      </c>
+      <c r="C76" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>287</v>
+      </c>
+      <c r="B77" t="s">
+        <v>288</v>
+      </c>
+      <c r="C77" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>290</v>
+      </c>
+      <c r="B78" t="s">
+        <v>291</v>
+      </c>
+      <c r="C78" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>293</v>
+      </c>
+      <c r="B79" t="s">
+        <v>294</v>
+      </c>
+      <c r="C79" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>296</v>
+      </c>
+      <c r="B80" t="s">
+        <v>297</v>
+      </c>
+      <c r="C80" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>299</v>
+      </c>
+      <c r="B81" t="s">
+        <v>300</v>
+      </c>
+      <c r="C81" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>302</v>
+      </c>
+      <c r="B82" t="s">
+        <v>303</v>
+      </c>
+      <c r="C82" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>305</v>
+      </c>
+      <c r="B83" t="s">
+        <v>306</v>
+      </c>
+      <c r="C83" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>308</v>
+      </c>
+      <c r="B84" t="s">
+        <v>309</v>
+      </c>
+      <c r="C84" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>311</v>
+      </c>
+      <c r="B85" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>314</v>
+      </c>
+      <c r="B86" t="s">
+        <v>315</v>
+      </c>
+      <c r="C86" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>317</v>
+      </c>
+      <c r="B87" t="s">
+        <v>318</v>
+      </c>
+      <c r="C87" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>320</v>
+      </c>
+      <c r="B88" t="s">
+        <v>321</v>
+      </c>
+      <c r="C88" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>323</v>
+      </c>
+      <c r="B89" t="s">
+        <v>324</v>
+      </c>
+      <c r="C89" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>326</v>
+      </c>
+      <c r="B90" t="s">
+        <v>327</v>
+      </c>
+      <c r="C90" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>329</v>
+      </c>
+      <c r="B91" t="s">
+        <v>330</v>
+      </c>
+      <c r="C91" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>332</v>
+      </c>
+      <c r="B92" t="s">
+        <v>333</v>
+      </c>
+      <c r="C92" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>335</v>
+      </c>
+      <c r="B93" t="s">
+        <v>336</v>
+      </c>
+      <c r="C93" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>338</v>
+      </c>
+      <c r="B94" t="s">
+        <v>339</v>
+      </c>
+      <c r="C94" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>341</v>
+      </c>
+      <c r="B95" t="s">
+        <v>342</v>
+      </c>
+      <c r="C95" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>344</v>
+      </c>
+      <c r="B96" t="s">
+        <v>345</v>
+      </c>
+      <c r="C96" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>347</v>
+      </c>
+      <c r="B97" t="s">
+        <v>348</v>
+      </c>
+      <c r="C97" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>350</v>
+      </c>
+      <c r="B98" t="s">
+        <v>351</v>
+      </c>
+      <c r="C98" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>353</v>
+      </c>
+      <c r="B99" t="s">
+        <v>354</v>
+      </c>
+      <c r="C99" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>356</v>
+      </c>
+      <c r="B100" t="s">
+        <v>357</v>
+      </c>
+      <c r="C100" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>359</v>
+      </c>
+      <c r="B101" t="s">
+        <v>360</v>
+      </c>
+      <c r="C101" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>362</v>
+      </c>
+      <c r="B102" t="s">
+        <v>363</v>
+      </c>
+      <c r="C102" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>365</v>
+      </c>
+      <c r="B103" t="s">
+        <v>366</v>
+      </c>
+      <c r="C103" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>368</v>
+      </c>
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+      <c r="C104" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>371</v>
+      </c>
+      <c r="B105" t="s">
+        <v>372</v>
+      </c>
+      <c r="C105" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>374</v>
+      </c>
+      <c r="B106" t="s">
+        <v>375</v>
+      </c>
+      <c r="C106" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>377</v>
+      </c>
+      <c r="B107" t="s">
+        <v>378</v>
+      </c>
+      <c r="C107" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>380</v>
+      </c>
+      <c r="B108" t="s">
+        <v>381</v>
+      </c>
+      <c r="C108" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>383</v>
+      </c>
+      <c r="B109" t="s">
+        <v>384</v>
+      </c>
+      <c r="C109" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>386</v>
+      </c>
+      <c r="B110" t="s">
+        <v>387</v>
+      </c>
+      <c r="C110" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>389</v>
+      </c>
+      <c r="B111" t="s">
+        <v>390</v>
+      </c>
+      <c r="C111" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" t="s">
+        <v>393</v>
+      </c>
+      <c r="C112" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>395</v>
+      </c>
+      <c r="B113" t="s">
+        <v>396</v>
+      </c>
+      <c r="C113" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>398</v>
+      </c>
+      <c r="B114" t="s">
+        <v>399</v>
+      </c>
+      <c r="C114" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>401</v>
+      </c>
+      <c r="B115" t="s">
+        <v>402</v>
+      </c>
+      <c r="C115" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>404</v>
+      </c>
+      <c r="B116" t="s">
+        <v>405</v>
+      </c>
+      <c r="C116" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>407</v>
+      </c>
+      <c r="B117" t="s">
+        <v>408</v>
+      </c>
+      <c r="C117" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>410</v>
+      </c>
+      <c r="B118" t="s">
+        <v>411</v>
+      </c>
+      <c r="C118" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>413</v>
+      </c>
+      <c r="B119" t="s">
+        <v>414</v>
+      </c>
+      <c r="C119" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>416</v>
+      </c>
+      <c r="B120" t="s">
+        <v>417</v>
+      </c>
+      <c r="C120" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>419</v>
+      </c>
+      <c r="B121" t="s">
+        <v>420</v>
+      </c>
+      <c r="C121" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>422</v>
+      </c>
+      <c r="B122" t="s">
+        <v>423</v>
+      </c>
+      <c r="C122" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>425</v>
+      </c>
+      <c r="B123" t="s">
+        <v>426</v>
+      </c>
+      <c r="C123" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>428</v>
+      </c>
+      <c r="B124" t="s">
+        <v>429</v>
+      </c>
+      <c r="C124" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>431</v>
+      </c>
+      <c r="B125" t="s">
+        <v>432</v>
+      </c>
+      <c r="C125" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>434</v>
+      </c>
+      <c r="B126" t="s">
+        <v>435</v>
+      </c>
+      <c r="C126" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>437</v>
+      </c>
+      <c r="B127" t="s">
+        <v>438</v>
+      </c>
+      <c r="C127" t="s">
+        <v>439</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>